<commit_message>
Commited on 20th April
</commit_message>
<xml_diff>
--- a/ocms/src/test/resources/TestData/OCMAgentInteractionReportData.xlsx
+++ b/ocms/src/test/resources/TestData/OCMAgentInteractionReportData.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BD42C0A-FA6E-4B61-8221-B7F2777EF3E0}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEC9D2E-4905-4B69-B008-5784EA500677}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1013,8 +1013,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE6D2C06-D0AE-4F83-B750-F2E25CDCB399}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>